<commit_message>
MeritOrderLänder hat die letzten Vereinfachungen erhalten und ist nun perfekt! PS: Noch kein Handel
</commit_message>
<xml_diff>
--- a/ErgebnisseDE.xlsx
+++ b/ErgebnisseDE.xlsx
@@ -473,7 +473,7 @@
         <v>7695.0</v>
       </c>
       <c r="B2">
-        <v>3155.1927670000005</v>
+        <v>2836.1927670000005</v>
       </c>
       <c r="C2">
         <v>0.0</v>
@@ -506,15 +506,15 @@
         <v>0.0</v>
       </c>
       <c r="M2">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N2">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>7438.401966000001</v>
+        <v>7119.401966000001</v>
       </c>
       <c r="B3">
         <v>0.0</v>
@@ -550,15 +550,15 @@
         <v>0.0</v>
       </c>
       <c r="M3">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N3">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>5634.985534000003</v>
+        <v>5315.985534000003</v>
       </c>
       <c r="B4">
         <v>0.0</v>
@@ -594,15 +594,15 @@
         <v>0.0</v>
       </c>
       <c r="M4">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N4">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>2885.5572329999995</v>
+        <v>2566.5572329999995</v>
       </c>
       <c r="B5">
         <v>0.0</v>
@@ -638,15 +638,15 @@
         <v>0.0</v>
       </c>
       <c r="M5">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N5">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>631.6072329999988</v>
+        <v>312.6072329999988</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -682,10 +682,10 @@
         <v>0.0</v>
       </c>
       <c r="M6">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N6">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -726,10 +726,10 @@
         <v>0.0</v>
       </c>
       <c r="M7">
-        <v>4370.0</v>
+        <v>3225.771698999997</v>
       </c>
       <c r="N7">
-        <v>635.7716989999972</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -770,10 +770,10 @@
         <v>0.0</v>
       </c>
       <c r="M8">
-        <v>1500.614465999999</v>
+        <v>1411.614465999999</v>
       </c>
       <c r="N8">
-        <v>1691.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -808,16 +808,16 @@
         <v>0.0</v>
       </c>
       <c r="K9">
-        <v>34372.0</v>
+        <v>36000.803301</v>
       </c>
       <c r="L9">
         <v>0.0</v>
       </c>
       <c r="M9">
-        <v>4370.0</v>
+        <v>961.1966990000001</v>
       </c>
       <c r="N9">
-        <v>0.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -858,10 +858,10 @@
         <v>112.2</v>
       </c>
       <c r="M10">
-        <v>2357.6269660000034</v>
+        <v>577.6269660000034</v>
       </c>
       <c r="N10">
-        <v>0.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -899,13 +899,13 @@
         <v>36367.009199</v>
       </c>
       <c r="L11">
-        <v>778.7212949999999</v>
+        <v>0.0</v>
       </c>
       <c r="M11">
-        <v>4370.0</v>
+        <v>4600.0</v>
       </c>
       <c r="N11">
-        <v>502.2695059999969</v>
+        <v>1050.990801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Constraint 1 zu Handel hinzugefügt
</commit_message>
<xml_diff>
--- a/ErgebnisseDE.xlsx
+++ b/ErgebnisseDE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Kernenergie</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Wasserkraft</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>NL</t>
   </si>
 </sst>
 </file>
@@ -418,13 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,13 +476,22 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>7695.0</v>
       </c>
       <c r="B2">
-        <v>2836.1927670000005</v>
+        <v>3755.1927670000005</v>
       </c>
       <c r="C2">
         <v>0.0</v>
@@ -506,18 +524,27 @@
         <v>0.0</v>
       </c>
       <c r="M2">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N2">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>1800.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
-        <v>7119.401966000001</v>
+        <v>7695.0</v>
       </c>
       <c r="B3">
-        <v>0.0</v>
+        <v>343.40196600000127</v>
       </c>
       <c r="C3">
         <v>0.0</v>
@@ -550,15 +577,24 @@
         <v>0.0</v>
       </c>
       <c r="M3">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N3">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>1800.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
-        <v>5315.985534000003</v>
+        <v>7695.0</v>
       </c>
       <c r="B4">
         <v>0.0</v>
@@ -594,15 +630,24 @@
         <v>0.0</v>
       </c>
       <c r="M4">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N4">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O4">
+        <v>0.0</v>
+      </c>
+      <c r="P4">
+        <v>339.9855340000031</v>
+      </c>
+      <c r="Q4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
-        <v>2566.5572329999995</v>
+        <v>3485.5572329999995</v>
       </c>
       <c r="B5">
         <v>0.0</v>
@@ -638,15 +683,24 @@
         <v>0.0</v>
       </c>
       <c r="M5">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N5">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O5">
+        <v>0.0</v>
+      </c>
+      <c r="P5">
+        <v>1800.0</v>
+      </c>
+      <c r="Q5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
-        <v>312.6072329999988</v>
+        <v>1231.6072329999988</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -682,15 +736,24 @@
         <v>0.0</v>
       </c>
       <c r="M6">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N6">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O6">
+        <v>0.0</v>
+      </c>
+      <c r="P6">
+        <v>1800.0</v>
+      </c>
+      <c r="Q6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
-        <v>0.0</v>
+        <v>3144.771698999997</v>
       </c>
       <c r="B7">
         <v>0.0</v>
@@ -726,13 +789,22 @@
         <v>0.0</v>
       </c>
       <c r="M7">
-        <v>3225.771698999997</v>
+        <v>4370.0</v>
       </c>
       <c r="N7">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O7">
+        <v>0.0</v>
+      </c>
+      <c r="P7">
+        <v>0.0</v>
+      </c>
+      <c r="Q7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>0.0</v>
       </c>
@@ -770,13 +842,22 @@
         <v>0.0</v>
       </c>
       <c r="M8">
-        <v>1411.614465999999</v>
+        <v>4370.0</v>
       </c>
       <c r="N8">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O8">
+        <v>0.0</v>
+      </c>
+      <c r="P8">
+        <v>0.0</v>
+      </c>
+      <c r="Q8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>0.0</v>
       </c>
@@ -814,13 +895,22 @@
         <v>0.0</v>
       </c>
       <c r="M9">
-        <v>961.1966990000001</v>
+        <v>4370.0</v>
       </c>
       <c r="N9">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O9">
+        <v>0.0</v>
+      </c>
+      <c r="P9">
+        <v>0.0</v>
+      </c>
+      <c r="Q9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>0.0</v>
       </c>
@@ -858,15 +948,24 @@
         <v>112.2</v>
       </c>
       <c r="M10">
-        <v>577.6269660000034</v>
+        <v>4370.0</v>
       </c>
       <c r="N10">
-        <v>1780.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>1691.0</v>
+      </c>
+      <c r="O10">
+        <v>0.0</v>
+      </c>
+      <c r="P10">
+        <v>0.0</v>
+      </c>
+      <c r="Q10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
-        <v>0.0</v>
+        <v>3011.269505999997</v>
       </c>
       <c r="B11">
         <v>0.0</v>
@@ -899,13 +998,764 @@
         <v>36367.009199</v>
       </c>
       <c r="L11">
-        <v>0.0</v>
+        <v>778.7212949999999</v>
       </c>
       <c r="M11">
-        <v>4600.0</v>
+        <v>4370.0</v>
       </c>
       <c r="N11">
-        <v>1050.990801</v>
+        <v>1691.0</v>
+      </c>
+      <c r="O11">
+        <v>0.0</v>
+      </c>
+      <c r="P11">
+        <v>0.0</v>
+      </c>
+      <c r="Q11">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>0.0</v>
+      </c>
+      <c r="B12">
+        <v>0.0</v>
+      </c>
+      <c r="C12">
+        <v>0.0</v>
+      </c>
+      <c r="D12">
+        <v>0.0</v>
+      </c>
+      <c r="E12">
+        <v>0.0</v>
+      </c>
+      <c r="F12">
+        <v>0.0</v>
+      </c>
+      <c r="G12">
+        <v>0.0</v>
+      </c>
+      <c r="H12">
+        <v>0.0</v>
+      </c>
+      <c r="I12">
+        <v>0.0</v>
+      </c>
+      <c r="J12">
+        <v>0.0</v>
+      </c>
+      <c r="K12">
+        <v>37709.010534</v>
+      </c>
+      <c r="L12">
+        <v>1828.592964</v>
+      </c>
+      <c r="M12">
+        <v>4370.0</v>
+      </c>
+      <c r="N12">
+        <v>1691.0</v>
+      </c>
+      <c r="O12">
+        <v>0.0</v>
+      </c>
+      <c r="P12">
+        <v>1334.396501999996</v>
+      </c>
+      <c r="Q12">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>0.0</v>
+      </c>
+      <c r="B13">
+        <v>0.0</v>
+      </c>
+      <c r="C13">
+        <v>0.0</v>
+      </c>
+      <c r="D13">
+        <v>0.0</v>
+      </c>
+      <c r="E13">
+        <v>0.0</v>
+      </c>
+      <c r="F13">
+        <v>0.0</v>
+      </c>
+      <c r="G13">
+        <v>0.0</v>
+      </c>
+      <c r="H13">
+        <v>0.0</v>
+      </c>
+      <c r="I13">
+        <v>0.0</v>
+      </c>
+      <c r="J13">
+        <v>0.0</v>
+      </c>
+      <c r="K13">
+        <v>40240.898034</v>
+      </c>
+      <c r="L13">
+        <v>2742.221295</v>
+      </c>
+      <c r="M13">
+        <v>4370.0</v>
+      </c>
+      <c r="N13">
+        <v>1691.0</v>
+      </c>
+      <c r="O13">
+        <v>0.0</v>
+      </c>
+      <c r="P13">
+        <v>844.880670999999</v>
+      </c>
+      <c r="Q13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <v>367.07832100000087</v>
+      </c>
+      <c r="B14">
+        <v>0.0</v>
+      </c>
+      <c r="C14">
+        <v>0.0</v>
+      </c>
+      <c r="D14">
+        <v>0.0</v>
+      </c>
+      <c r="E14">
+        <v>0.0</v>
+      </c>
+      <c r="F14">
+        <v>0.0</v>
+      </c>
+      <c r="G14">
+        <v>0.0</v>
+      </c>
+      <c r="H14">
+        <v>0.0</v>
+      </c>
+      <c r="I14">
+        <v>0.0</v>
+      </c>
+      <c r="J14">
+        <v>0.0</v>
+      </c>
+      <c r="K14">
+        <v>40451.607233</v>
+      </c>
+      <c r="L14">
+        <v>2981.314446</v>
+      </c>
+      <c r="M14">
+        <v>4370.0</v>
+      </c>
+      <c r="N14">
+        <v>1691.0</v>
+      </c>
+      <c r="O14">
+        <v>0.0</v>
+      </c>
+      <c r="P14">
+        <v>1800.0</v>
+      </c>
+      <c r="Q14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15">
+        <v>0.0</v>
+      </c>
+      <c r="B15">
+        <v>0.0</v>
+      </c>
+      <c r="C15">
+        <v>0.0</v>
+      </c>
+      <c r="D15">
+        <v>0.0</v>
+      </c>
+      <c r="E15">
+        <v>0.0</v>
+      </c>
+      <c r="F15">
+        <v>0.0</v>
+      </c>
+      <c r="G15">
+        <v>0.0</v>
+      </c>
+      <c r="H15">
+        <v>0.0</v>
+      </c>
+      <c r="I15">
+        <v>0.0</v>
+      </c>
+      <c r="J15">
+        <v>0.0</v>
+      </c>
+      <c r="K15">
+        <v>41076.973034</v>
+      </c>
+      <c r="L15">
+        <v>2679.44259</v>
+      </c>
+      <c r="M15">
+        <v>4370.0</v>
+      </c>
+      <c r="N15">
+        <v>1691.0</v>
+      </c>
+      <c r="O15">
+        <v>0.0</v>
+      </c>
+      <c r="P15">
+        <v>1414.5843759999989</v>
+      </c>
+      <c r="Q15">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16">
+        <v>0.0</v>
+      </c>
+      <c r="B16">
+        <v>0.0</v>
+      </c>
+      <c r="C16">
+        <v>0.0</v>
+      </c>
+      <c r="D16">
+        <v>0.0</v>
+      </c>
+      <c r="E16">
+        <v>0.0</v>
+      </c>
+      <c r="F16">
+        <v>0.0</v>
+      </c>
+      <c r="G16">
+        <v>0.0</v>
+      </c>
+      <c r="H16">
+        <v>0.0</v>
+      </c>
+      <c r="I16">
+        <v>0.0</v>
+      </c>
+      <c r="J16">
+        <v>0.0</v>
+      </c>
+      <c r="K16">
+        <v>41542.335534</v>
+      </c>
+      <c r="L16">
+        <v>1732.421295</v>
+      </c>
+      <c r="M16">
+        <v>4370.0</v>
+      </c>
+      <c r="N16">
+        <v>1691.0</v>
+      </c>
+      <c r="O16">
+        <v>0.0</v>
+      </c>
+      <c r="P16">
+        <v>1659.243171000002</v>
+      </c>
+      <c r="Q16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17">
+        <v>4849.680070000002</v>
+      </c>
+      <c r="B17">
+        <v>0.0</v>
+      </c>
+      <c r="C17">
+        <v>0.0</v>
+      </c>
+      <c r="D17">
+        <v>0.0</v>
+      </c>
+      <c r="E17">
+        <v>0.0</v>
+      </c>
+      <c r="F17">
+        <v>0.0</v>
+      </c>
+      <c r="G17">
+        <v>0.0</v>
+      </c>
+      <c r="H17">
+        <v>0.0</v>
+      </c>
+      <c r="I17">
+        <v>0.0</v>
+      </c>
+      <c r="J17">
+        <v>0.0</v>
+      </c>
+      <c r="K17">
+        <v>41520.926966</v>
+      </c>
+      <c r="L17">
+        <v>594.392964</v>
+      </c>
+      <c r="M17">
+        <v>4370.0</v>
+      </c>
+      <c r="N17">
+        <v>1691.0</v>
+      </c>
+      <c r="O17">
+        <v>0.0</v>
+      </c>
+      <c r="P17">
+        <v>0.0</v>
+      </c>
+      <c r="Q17">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18">
+        <v>2368.462293000004</v>
+      </c>
+      <c r="B18">
+        <v>0.0</v>
+      </c>
+      <c r="C18">
+        <v>0.0</v>
+      </c>
+      <c r="D18">
+        <v>0.0</v>
+      </c>
+      <c r="E18">
+        <v>0.0</v>
+      </c>
+      <c r="F18">
+        <v>0.0</v>
+      </c>
+      <c r="G18">
+        <v>0.0</v>
+      </c>
+      <c r="H18">
+        <v>0.0</v>
+      </c>
+      <c r="I18">
+        <v>0.0</v>
+      </c>
+      <c r="J18">
+        <v>0.0</v>
+      </c>
+      <c r="K18">
+        <v>42767.151966</v>
+      </c>
+      <c r="L18">
+        <v>29.385741</v>
+      </c>
+      <c r="M18">
+        <v>4370.0</v>
+      </c>
+      <c r="N18">
+        <v>1691.0</v>
+      </c>
+      <c r="O18">
+        <v>0.0</v>
+      </c>
+      <c r="P18">
+        <v>1800.0</v>
+      </c>
+      <c r="Q18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19">
+        <v>4895.537500000006</v>
+      </c>
+      <c r="B19">
+        <v>0.0</v>
+      </c>
+      <c r="C19">
+        <v>0.0</v>
+      </c>
+      <c r="D19">
+        <v>0.0</v>
+      </c>
+      <c r="E19">
+        <v>0.0</v>
+      </c>
+      <c r="F19">
+        <v>0.0</v>
+      </c>
+      <c r="G19">
+        <v>0.0</v>
+      </c>
+      <c r="H19">
+        <v>0.0</v>
+      </c>
+      <c r="I19">
+        <v>0.0</v>
+      </c>
+      <c r="J19">
+        <v>0.0</v>
+      </c>
+      <c r="K19">
+        <v>43436.462499999994</v>
+      </c>
+      <c r="L19">
+        <v>0.0</v>
+      </c>
+      <c r="M19">
+        <v>4370.0</v>
+      </c>
+      <c r="N19">
+        <v>1691.0</v>
+      </c>
+      <c r="O19">
+        <v>0.0</v>
+      </c>
+      <c r="P19">
+        <v>1800.0</v>
+      </c>
+      <c r="Q19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20">
+        <v>5494.946699</v>
+      </c>
+      <c r="B20">
+        <v>0.0</v>
+      </c>
+      <c r="C20">
+        <v>0.0</v>
+      </c>
+      <c r="D20">
+        <v>0.0</v>
+      </c>
+      <c r="E20">
+        <v>0.0</v>
+      </c>
+      <c r="F20">
+        <v>0.0</v>
+      </c>
+      <c r="G20">
+        <v>0.0</v>
+      </c>
+      <c r="H20">
+        <v>0.0</v>
+      </c>
+      <c r="I20">
+        <v>0.0</v>
+      </c>
+      <c r="J20">
+        <v>0.0</v>
+      </c>
+      <c r="K20">
+        <v>43415.053301</v>
+      </c>
+      <c r="L20">
+        <v>0.0</v>
+      </c>
+      <c r="M20">
+        <v>4370.0</v>
+      </c>
+      <c r="N20">
+        <v>1691.0</v>
+      </c>
+      <c r="O20">
+        <v>0.0</v>
+      </c>
+      <c r="P20">
+        <v>1800.0</v>
+      </c>
+      <c r="Q20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21">
+        <v>5290.503301000004</v>
+      </c>
+      <c r="B21">
+        <v>0.0</v>
+      </c>
+      <c r="C21">
+        <v>0.0</v>
+      </c>
+      <c r="D21">
+        <v>0.0</v>
+      </c>
+      <c r="E21">
+        <v>0.0</v>
+      </c>
+      <c r="F21">
+        <v>0.0</v>
+      </c>
+      <c r="G21">
+        <v>0.0</v>
+      </c>
+      <c r="H21">
+        <v>0.0</v>
+      </c>
+      <c r="I21">
+        <v>0.0</v>
+      </c>
+      <c r="J21">
+        <v>0.0</v>
+      </c>
+      <c r="K21">
+        <v>43063.496698999996</v>
+      </c>
+      <c r="L21">
+        <v>0.0</v>
+      </c>
+      <c r="M21">
+        <v>4370.0</v>
+      </c>
+      <c r="N21">
+        <v>1691.0</v>
+      </c>
+      <c r="O21">
+        <v>0.0</v>
+      </c>
+      <c r="P21">
+        <v>1800.0</v>
+      </c>
+      <c r="Q21">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>3108.165801000003</v>
+      </c>
+      <c r="B22">
+        <v>0.0</v>
+      </c>
+      <c r="C22">
+        <v>0.0</v>
+      </c>
+      <c r="D22">
+        <v>0.0</v>
+      </c>
+      <c r="E22">
+        <v>0.0</v>
+      </c>
+      <c r="F22">
+        <v>0.0</v>
+      </c>
+      <c r="G22">
+        <v>0.0</v>
+      </c>
+      <c r="H22">
+        <v>0.0</v>
+      </c>
+      <c r="I22">
+        <v>0.0</v>
+      </c>
+      <c r="J22">
+        <v>0.0</v>
+      </c>
+      <c r="K22">
+        <v>43039.834199</v>
+      </c>
+      <c r="L22">
+        <v>0.0</v>
+      </c>
+      <c r="M22">
+        <v>4370.0</v>
+      </c>
+      <c r="N22">
+        <v>1691.0</v>
+      </c>
+      <c r="O22">
+        <v>0.0</v>
+      </c>
+      <c r="P22">
+        <v>1800.0</v>
+      </c>
+      <c r="Q22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <v>5281.684199000003</v>
+      </c>
+      <c r="B23">
+        <v>0.0</v>
+      </c>
+      <c r="C23">
+        <v>0.0</v>
+      </c>
+      <c r="D23">
+        <v>0.0</v>
+      </c>
+      <c r="E23">
+        <v>0.0</v>
+      </c>
+      <c r="F23">
+        <v>0.0</v>
+      </c>
+      <c r="G23">
+        <v>0.0</v>
+      </c>
+      <c r="H23">
+        <v>0.0</v>
+      </c>
+      <c r="I23">
+        <v>0.0</v>
+      </c>
+      <c r="J23">
+        <v>0.0</v>
+      </c>
+      <c r="K23">
+        <v>42555.315801</v>
+      </c>
+      <c r="L23">
+        <v>0.0</v>
+      </c>
+      <c r="M23">
+        <v>4370.0</v>
+      </c>
+      <c r="N23">
+        <v>1691.0</v>
+      </c>
+      <c r="O23">
+        <v>0.0</v>
+      </c>
+      <c r="P23">
+        <v>0.0</v>
+      </c>
+      <c r="Q23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <v>5501.862499999996</v>
+      </c>
+      <c r="B24">
+        <v>0.0</v>
+      </c>
+      <c r="C24">
+        <v>0.0</v>
+      </c>
+      <c r="D24">
+        <v>0.0</v>
+      </c>
+      <c r="E24">
+        <v>0.0</v>
+      </c>
+      <c r="F24">
+        <v>0.0</v>
+      </c>
+      <c r="G24">
+        <v>0.0</v>
+      </c>
+      <c r="H24">
+        <v>0.0</v>
+      </c>
+      <c r="I24">
+        <v>0.0</v>
+      </c>
+      <c r="J24">
+        <v>0.0</v>
+      </c>
+      <c r="K24">
+        <v>41496.137500000004</v>
+      </c>
+      <c r="L24">
+        <v>0.0</v>
+      </c>
+      <c r="M24">
+        <v>4370.0</v>
+      </c>
+      <c r="N24">
+        <v>1691.0</v>
+      </c>
+      <c r="O24">
+        <v>0.0</v>
+      </c>
+      <c r="P24">
+        <v>0.0</v>
+      </c>
+      <c r="Q24">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>0.0</v>
+      </c>
+      <c r="B25">
+        <v>0.0</v>
+      </c>
+      <c r="C25">
+        <v>0.0</v>
+      </c>
+      <c r="D25">
+        <v>0.0</v>
+      </c>
+      <c r="E25">
+        <v>0.0</v>
+      </c>
+      <c r="F25">
+        <v>0.0</v>
+      </c>
+      <c r="G25">
+        <v>0.0</v>
+      </c>
+      <c r="H25">
+        <v>0.0</v>
+      </c>
+      <c r="I25">
+        <v>0.0</v>
+      </c>
+      <c r="J25">
+        <v>0.0</v>
+      </c>
+      <c r="K25">
+        <v>41087.114466</v>
+      </c>
+      <c r="L25">
+        <v>0.0</v>
+      </c>
+      <c r="M25">
+        <v>4370.0</v>
+      </c>
+      <c r="N25">
+        <v>1691.0</v>
+      </c>
+      <c r="O25">
+        <v>0.0</v>
+      </c>
+      <c r="P25">
+        <v>1344.885534000001</v>
+      </c>
+      <c r="Q25">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ergebnisausgabe angepasst -> Alles wird in einer Exceltabelle ausgegeben statt in verschiedenen je für ein Land eine
</commit_message>
<xml_diff>
--- a/ErgebnisseDE.xlsx
+++ b/ErgebnisseDE.xlsx
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,7 +491,7 @@
         <v>7695.0</v>
       </c>
       <c r="B2">
-        <v>3857.1927670000005</v>
+        <v>3935.1927670000005</v>
       </c>
       <c r="C2">
         <v>0.0</v>
@@ -533,7 +533,7 @@
         <v>0.0</v>
       </c>
       <c r="P2">
-        <v>1620.0</v>
+        <v>1800.0</v>
       </c>
       <c r="Q2">
         <v>0.0</v>
@@ -544,7 +544,7 @@
         <v>7695.0</v>
       </c>
       <c r="B3">
-        <v>445.40196600000127</v>
+        <v>523.4019660000013</v>
       </c>
       <c r="C3">
         <v>0.0</v>
@@ -586,7 +586,7 @@
         <v>0.0</v>
       </c>
       <c r="P3">
-        <v>1620.0</v>
+        <v>1800.0</v>
       </c>
       <c r="Q3">
         <v>0.0</v>
@@ -639,7 +639,7 @@
         <v>0.0</v>
       </c>
       <c r="P4">
-        <v>111.09503777777718</v>
+        <v>377.7617044444414</v>
       </c>
       <c r="Q4">
         <v>0.0</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>5045.5572329999995</v>
+        <v>5285.5572329999995</v>
       </c>
       <c r="B5">
         <v>0.0</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>2791.607232999999</v>
+        <v>3031.607232999999</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>1104.7716989999972</v>
+        <v>1344.7716989999972</v>
       </c>
       <c r="B7">
         <v>0.0</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11">
-        <v>971.2695059999969</v>
+        <v>1211.269505999997</v>
       </c>
       <c r="B11">
         <v>0.0</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <v>1094.396501999996</v>
+        <v>1334.396501999996</v>
       </c>
       <c r="B12">
         <v>0.0</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13">
-        <v>604.880670999999</v>
+        <v>844.880670999999</v>
       </c>
       <c r="B13">
         <v>0.0</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14">
-        <v>1927.0783210000009</v>
+        <v>2167.078321000001</v>
       </c>
       <c r="B14">
         <v>0.0</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15">
-        <v>1174.5843759999989</v>
+        <v>1414.5843759999989</v>
       </c>
       <c r="B15">
         <v>0.0</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16">
-        <v>1419.243171000002</v>
+        <v>1659.243171000002</v>
       </c>
       <c r="B16">
         <v>0.0</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17">
-        <v>2809.680070000002</v>
+        <v>3049.680070000002</v>
       </c>
       <c r="B17">
         <v>0.0</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18">
-        <v>3928.462293000004</v>
+        <v>4168.462293000004</v>
       </c>
       <c r="B18">
         <v>0.0</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19">
-        <v>6455.537500000006</v>
+        <v>6695.537500000006</v>
       </c>
       <c r="B19">
         <v>0.0</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20">
-        <v>7054.946699</v>
+        <v>7294.946699</v>
       </c>
       <c r="B20">
         <v>0.0</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21">
-        <v>6850.503301000004</v>
+        <v>7090.503301000004</v>
       </c>
       <c r="B21">
         <v>0.0</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22">
-        <v>4668.165801000003</v>
+        <v>4908.165801000003</v>
       </c>
       <c r="B22">
         <v>0.0</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23">
-        <v>3241.684199000003</v>
+        <v>3481.684199000003</v>
       </c>
       <c r="B23">
         <v>0.0</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24">
-        <v>3461.8624999999956</v>
+        <v>3701.8624999999956</v>
       </c>
       <c r="B24">
         <v>0.0</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
-        <v>1104.885534000001</v>
+        <v>1344.885534000001</v>
       </c>
       <c r="B25">
         <v>0.0</v>
@@ -1755,1278 +1755,6 @@
         <v>0.0</v>
       </c>
       <c r="Q25">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26">
-        <v>1429.0875000000015</v>
-      </c>
-      <c r="B26">
-        <v>0.0</v>
-      </c>
-      <c r="C26">
-        <v>0.0</v>
-      </c>
-      <c r="D26">
-        <v>0.0</v>
-      </c>
-      <c r="E26">
-        <v>0.0</v>
-      </c>
-      <c r="F26">
-        <v>0.0</v>
-      </c>
-      <c r="G26">
-        <v>0.0</v>
-      </c>
-      <c r="H26">
-        <v>0.0</v>
-      </c>
-      <c r="I26">
-        <v>0.0</v>
-      </c>
-      <c r="J26">
-        <v>0.0</v>
-      </c>
-      <c r="K26">
-        <v>38987.9125</v>
-      </c>
-      <c r="L26">
-        <v>0.0</v>
-      </c>
-      <c r="M26">
-        <v>4370.0</v>
-      </c>
-      <c r="N26">
-        <v>1691.0</v>
-      </c>
-      <c r="O26">
-        <v>0.0</v>
-      </c>
-      <c r="P26">
-        <v>0.0</v>
-      </c>
-      <c r="Q26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27">
-        <v>996.7874999999985</v>
-      </c>
-      <c r="B27">
-        <v>0.0</v>
-      </c>
-      <c r="C27">
-        <v>0.0</v>
-      </c>
-      <c r="D27">
-        <v>0.0</v>
-      </c>
-      <c r="E27">
-        <v>0.0</v>
-      </c>
-      <c r="F27">
-        <v>0.0</v>
-      </c>
-      <c r="G27">
-        <v>0.0</v>
-      </c>
-      <c r="H27">
-        <v>0.0</v>
-      </c>
-      <c r="I27">
-        <v>0.0</v>
-      </c>
-      <c r="J27">
-        <v>0.0</v>
-      </c>
-      <c r="K27">
-        <v>37915.2125</v>
-      </c>
-      <c r="L27">
-        <v>0.0</v>
-      </c>
-      <c r="M27">
-        <v>4370.0</v>
-      </c>
-      <c r="N27">
-        <v>1691.0</v>
-      </c>
-      <c r="O27">
-        <v>0.0</v>
-      </c>
-      <c r="P27">
-        <v>0.0</v>
-      </c>
-      <c r="Q27">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28">
-        <v>1112.5052670000005</v>
-      </c>
-      <c r="B28">
-        <v>0.0</v>
-      </c>
-      <c r="C28">
-        <v>0.0</v>
-      </c>
-      <c r="D28">
-        <v>0.0</v>
-      </c>
-      <c r="E28">
-        <v>0.0</v>
-      </c>
-      <c r="F28">
-        <v>0.0</v>
-      </c>
-      <c r="G28">
-        <v>0.0</v>
-      </c>
-      <c r="H28">
-        <v>0.0</v>
-      </c>
-      <c r="I28">
-        <v>0.0</v>
-      </c>
-      <c r="J28">
-        <v>0.0</v>
-      </c>
-      <c r="K28">
-        <v>37304.494733</v>
-      </c>
-      <c r="L28">
-        <v>0.0</v>
-      </c>
-      <c r="M28">
-        <v>4370.0</v>
-      </c>
-      <c r="N28">
-        <v>1691.0</v>
-      </c>
-      <c r="O28">
-        <v>0.0</v>
-      </c>
-      <c r="P28">
-        <v>0.0</v>
-      </c>
-      <c r="Q28">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29">
-        <v>1316.6875</v>
-      </c>
-      <c r="B29">
-        <v>0.0</v>
-      </c>
-      <c r="C29">
-        <v>0.0</v>
-      </c>
-      <c r="D29">
-        <v>0.0</v>
-      </c>
-      <c r="E29">
-        <v>0.0</v>
-      </c>
-      <c r="F29">
-        <v>0.0</v>
-      </c>
-      <c r="G29">
-        <v>0.0</v>
-      </c>
-      <c r="H29">
-        <v>0.0</v>
-      </c>
-      <c r="I29">
-        <v>0.0</v>
-      </c>
-      <c r="J29">
-        <v>0.0</v>
-      </c>
-      <c r="K29">
-        <v>36716.3125</v>
-      </c>
-      <c r="L29">
-        <v>0.0</v>
-      </c>
-      <c r="M29">
-        <v>4370.0</v>
-      </c>
-      <c r="N29">
-        <v>1691.0</v>
-      </c>
-      <c r="O29">
-        <v>0.0</v>
-      </c>
-      <c r="P29">
-        <v>0.0</v>
-      </c>
-      <c r="Q29">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30">
-        <v>2567.1427669999975</v>
-      </c>
-      <c r="B30">
-        <v>0.0</v>
-      </c>
-      <c r="C30">
-        <v>0.0</v>
-      </c>
-      <c r="D30">
-        <v>0.0</v>
-      </c>
-      <c r="E30">
-        <v>0.0</v>
-      </c>
-      <c r="F30">
-        <v>0.0</v>
-      </c>
-      <c r="G30">
-        <v>0.0</v>
-      </c>
-      <c r="H30">
-        <v>0.0</v>
-      </c>
-      <c r="I30">
-        <v>0.0</v>
-      </c>
-      <c r="J30">
-        <v>0.0</v>
-      </c>
-      <c r="K30">
-        <v>37138.857233</v>
-      </c>
-      <c r="L30">
-        <v>0.0</v>
-      </c>
-      <c r="M30">
-        <v>4370.0</v>
-      </c>
-      <c r="N30">
-        <v>1691.0</v>
-      </c>
-      <c r="O30">
-        <v>0.0</v>
-      </c>
-      <c r="P30">
-        <v>0.0</v>
-      </c>
-      <c r="Q30">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31">
-        <v>4206.214465999998</v>
-      </c>
-      <c r="B31">
-        <v>0.0</v>
-      </c>
-      <c r="C31">
-        <v>0.0</v>
-      </c>
-      <c r="D31">
-        <v>0.0</v>
-      </c>
-      <c r="E31">
-        <v>0.0</v>
-      </c>
-      <c r="F31">
-        <v>0.0</v>
-      </c>
-      <c r="G31">
-        <v>0.0</v>
-      </c>
-      <c r="H31">
-        <v>0.0</v>
-      </c>
-      <c r="I31">
-        <v>0.0</v>
-      </c>
-      <c r="J31">
-        <v>0.0</v>
-      </c>
-      <c r="K31">
-        <v>38355.785534</v>
-      </c>
-      <c r="L31">
-        <v>0.0</v>
-      </c>
-      <c r="M31">
-        <v>4370.0</v>
-      </c>
-      <c r="N31">
-        <v>1691.0</v>
-      </c>
-      <c r="O31">
-        <v>0.0</v>
-      </c>
-      <c r="P31">
-        <v>0.0</v>
-      </c>
-      <c r="Q31">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32">
-        <v>7695.0</v>
-      </c>
-      <c r="B32">
-        <v>0.0</v>
-      </c>
-      <c r="C32">
-        <v>0.0</v>
-      </c>
-      <c r="D32">
-        <v>0.0</v>
-      </c>
-      <c r="E32">
-        <v>0.0</v>
-      </c>
-      <c r="F32">
-        <v>0.0</v>
-      </c>
-      <c r="G32">
-        <v>0.0</v>
-      </c>
-      <c r="H32">
-        <v>0.0</v>
-      </c>
-      <c r="I32">
-        <v>0.0</v>
-      </c>
-      <c r="J32">
-        <v>0.0</v>
-      </c>
-      <c r="K32">
-        <v>39613.278301000006</v>
-      </c>
-      <c r="L32">
-        <v>0.0</v>
-      </c>
-      <c r="M32">
-        <v>4370.0</v>
-      </c>
-      <c r="N32">
-        <v>1691.0</v>
-      </c>
-      <c r="O32">
-        <v>0.0</v>
-      </c>
-      <c r="P32">
-        <v>1244.135221111108</v>
-      </c>
-      <c r="Q32">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33">
-        <v>7695.0</v>
-      </c>
-      <c r="B33">
-        <v>4871.5341990000015</v>
-      </c>
-      <c r="C33">
-        <v>0.0</v>
-      </c>
-      <c r="D33">
-        <v>0.0</v>
-      </c>
-      <c r="E33">
-        <v>0.0</v>
-      </c>
-      <c r="F33">
-        <v>0.0</v>
-      </c>
-      <c r="G33">
-        <v>0.0</v>
-      </c>
-      <c r="H33">
-        <v>0.0</v>
-      </c>
-      <c r="I33">
-        <v>0.0</v>
-      </c>
-      <c r="J33">
-        <v>0.0</v>
-      </c>
-      <c r="K33">
-        <v>39810.465801</v>
-      </c>
-      <c r="L33">
-        <v>0.0</v>
-      </c>
-      <c r="M33">
-        <v>4370.0</v>
-      </c>
-      <c r="N33">
-        <v>1691.0</v>
-      </c>
-      <c r="O33">
-        <v>0.0</v>
-      </c>
-      <c r="P33">
-        <v>1620.0</v>
-      </c>
-      <c r="Q33">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34">
-        <v>7695.0</v>
-      </c>
-      <c r="B34">
-        <v>9347.871077999996</v>
-      </c>
-      <c r="C34">
-        <v>0.0</v>
-      </c>
-      <c r="D34">
-        <v>0.0</v>
-      </c>
-      <c r="E34">
-        <v>0.0</v>
-      </c>
-      <c r="F34">
-        <v>0.0</v>
-      </c>
-      <c r="G34">
-        <v>0.0</v>
-      </c>
-      <c r="H34">
-        <v>0.0</v>
-      </c>
-      <c r="I34">
-        <v>0.0</v>
-      </c>
-      <c r="J34">
-        <v>0.0</v>
-      </c>
-      <c r="K34">
-        <v>38409.871699</v>
-      </c>
-      <c r="L34">
-        <v>144.257223</v>
-      </c>
-      <c r="M34">
-        <v>4370.0</v>
-      </c>
-      <c r="N34">
-        <v>1691.0</v>
-      </c>
-      <c r="O34">
-        <v>0.0</v>
-      </c>
-      <c r="P34">
-        <v>1620.0</v>
-      </c>
-      <c r="Q34">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35">
-        <v>7695.0</v>
-      </c>
-      <c r="B35">
-        <v>10629.482056000008</v>
-      </c>
-      <c r="C35">
-        <v>0.0</v>
-      </c>
-      <c r="D35">
-        <v>0.0</v>
-      </c>
-      <c r="E35">
-        <v>0.0</v>
-      </c>
-      <c r="F35">
-        <v>0.0</v>
-      </c>
-      <c r="G35">
-        <v>0.0</v>
-      </c>
-      <c r="H35">
-        <v>0.0</v>
-      </c>
-      <c r="I35">
-        <v>0.0</v>
-      </c>
-      <c r="J35">
-        <v>0.0</v>
-      </c>
-      <c r="K35">
-        <v>37172.660533999995</v>
-      </c>
-      <c r="L35">
-        <v>1976.85741</v>
-      </c>
-      <c r="M35">
-        <v>4370.0</v>
-      </c>
-      <c r="N35">
-        <v>1691.0</v>
-      </c>
-      <c r="O35">
-        <v>0.0</v>
-      </c>
-      <c r="P35">
-        <v>1620.0</v>
-      </c>
-      <c r="Q35">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36">
-        <v>7695.0</v>
-      </c>
-      <c r="B36">
-        <v>9191.530444000004</v>
-      </c>
-      <c r="C36">
-        <v>0.0</v>
-      </c>
-      <c r="D36">
-        <v>0.0</v>
-      </c>
-      <c r="E36">
-        <v>0.0</v>
-      </c>
-      <c r="F36">
-        <v>0.0</v>
-      </c>
-      <c r="G36">
-        <v>0.0</v>
-      </c>
-      <c r="H36">
-        <v>0.0</v>
-      </c>
-      <c r="I36">
-        <v>0.0</v>
-      </c>
-      <c r="J36">
-        <v>0.0</v>
-      </c>
-      <c r="K36">
-        <v>36472.926966</v>
-      </c>
-      <c r="L36">
-        <v>5540.54259</v>
-      </c>
-      <c r="M36">
-        <v>4370.0</v>
-      </c>
-      <c r="N36">
-        <v>1691.0</v>
-      </c>
-      <c r="O36">
-        <v>0.0</v>
-      </c>
-      <c r="P36">
-        <v>1620.0</v>
-      </c>
-      <c r="Q36">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37">
-        <v>7695.0</v>
-      </c>
-      <c r="B37">
-        <v>7642.510720999999</v>
-      </c>
-      <c r="C37">
-        <v>0.0</v>
-      </c>
-      <c r="D37">
-        <v>0.0</v>
-      </c>
-      <c r="E37">
-        <v>0.0</v>
-      </c>
-      <c r="F37">
-        <v>0.0</v>
-      </c>
-      <c r="G37">
-        <v>0.0</v>
-      </c>
-      <c r="H37">
-        <v>0.0</v>
-      </c>
-      <c r="I37">
-        <v>0.0</v>
-      </c>
-      <c r="J37">
-        <v>0.0</v>
-      </c>
-      <c r="K37">
-        <v>36275.739466</v>
-      </c>
-      <c r="L37">
-        <v>8461.749812999999</v>
-      </c>
-      <c r="M37">
-        <v>4370.0</v>
-      </c>
-      <c r="N37">
-        <v>1691.0</v>
-      </c>
-      <c r="O37">
-        <v>0.0</v>
-      </c>
-      <c r="P37">
-        <v>1620.0</v>
-      </c>
-      <c r="Q37">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38">
-        <v>7695.0</v>
-      </c>
-      <c r="B38">
-        <v>7206.858775000001</v>
-      </c>
-      <c r="C38">
-        <v>0.0</v>
-      </c>
-      <c r="D38">
-        <v>0.0</v>
-      </c>
-      <c r="E38">
-        <v>0.0</v>
-      </c>
-      <c r="F38">
-        <v>0.0</v>
-      </c>
-      <c r="G38">
-        <v>0.0</v>
-      </c>
-      <c r="H38">
-        <v>0.0</v>
-      </c>
-      <c r="I38">
-        <v>0.0</v>
-      </c>
-      <c r="J38">
-        <v>0.0</v>
-      </c>
-      <c r="K38">
-        <v>36188.976966</v>
-      </c>
-      <c r="L38">
-        <v>9255.164259</v>
-      </c>
-      <c r="M38">
-        <v>4370.0</v>
-      </c>
-      <c r="N38">
-        <v>1691.0</v>
-      </c>
-      <c r="O38">
-        <v>0.0</v>
-      </c>
-      <c r="P38">
-        <v>1620.0</v>
-      </c>
-      <c r="Q38">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39">
-        <v>7695.0</v>
-      </c>
-      <c r="B39">
-        <v>7959.916195000005</v>
-      </c>
-      <c r="C39">
-        <v>0.0</v>
-      </c>
-      <c r="D39">
-        <v>0.0</v>
-      </c>
-      <c r="E39">
-        <v>0.0</v>
-      </c>
-      <c r="F39">
-        <v>0.0</v>
-      </c>
-      <c r="G39">
-        <v>0.0</v>
-      </c>
-      <c r="H39">
-        <v>0.0</v>
-      </c>
-      <c r="I39">
-        <v>0.0</v>
-      </c>
-      <c r="J39">
-        <v>0.0</v>
-      </c>
-      <c r="K39">
-        <v>35458.819733</v>
-      </c>
-      <c r="L39">
-        <v>8376.264072</v>
-      </c>
-      <c r="M39">
-        <v>4370.0</v>
-      </c>
-      <c r="N39">
-        <v>1691.0</v>
-      </c>
-      <c r="O39">
-        <v>0.0</v>
-      </c>
-      <c r="P39">
-        <v>1620.0</v>
-      </c>
-      <c r="Q39">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40">
-        <v>7695.0</v>
-      </c>
-      <c r="B40">
-        <v>11334.533992000004</v>
-      </c>
-      <c r="C40">
-        <v>0.0</v>
-      </c>
-      <c r="D40">
-        <v>0.0</v>
-      </c>
-      <c r="E40">
-        <v>0.0</v>
-      </c>
-      <c r="F40">
-        <v>0.0</v>
-      </c>
-      <c r="G40">
-        <v>0.0</v>
-      </c>
-      <c r="H40">
-        <v>0.0</v>
-      </c>
-      <c r="I40">
-        <v>0.0</v>
-      </c>
-      <c r="J40">
-        <v>0.0</v>
-      </c>
-      <c r="K40">
-        <v>33193.980267</v>
-      </c>
-      <c r="L40">
-        <v>5695.485741</v>
-      </c>
-      <c r="M40">
-        <v>4370.0</v>
-      </c>
-      <c r="N40">
-        <v>1691.0</v>
-      </c>
-      <c r="O40">
-        <v>0.0</v>
-      </c>
-      <c r="P40">
-        <v>1620.0</v>
-      </c>
-      <c r="Q40">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="A41">
-        <v>7695.0</v>
-      </c>
-      <c r="B41">
-        <v>13395.0</v>
-      </c>
-      <c r="C41">
-        <v>3230.0</v>
-      </c>
-      <c r="D41">
-        <v>1056.6605640000053</v>
-      </c>
-      <c r="E41">
-        <v>0.0</v>
-      </c>
-      <c r="F41">
-        <v>0.0</v>
-      </c>
-      <c r="G41">
-        <v>0.0</v>
-      </c>
-      <c r="H41">
-        <v>0.0</v>
-      </c>
-      <c r="I41">
-        <v>0.0</v>
-      </c>
-      <c r="J41">
-        <v>0.0</v>
-      </c>
-      <c r="K41">
-        <v>30614.767766999998</v>
-      </c>
-      <c r="L41">
-        <v>2003.5716690000002</v>
-      </c>
-      <c r="M41">
-        <v>4370.0</v>
-      </c>
-      <c r="N41">
-        <v>1691.0</v>
-      </c>
-      <c r="O41">
-        <v>0.0</v>
-      </c>
-      <c r="P41">
-        <v>1620.0</v>
-      </c>
-      <c r="Q41">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="A42">
-        <v>7695.0</v>
-      </c>
-      <c r="B42">
-        <v>13395.0</v>
-      </c>
-      <c r="C42">
-        <v>3230.0</v>
-      </c>
-      <c r="D42">
-        <v>2850.0</v>
-      </c>
-      <c r="E42">
-        <v>2851.7462749999977</v>
-      </c>
-      <c r="F42">
-        <v>0.0</v>
-      </c>
-      <c r="G42">
-        <v>0.0</v>
-      </c>
-      <c r="H42">
-        <v>0.0</v>
-      </c>
-      <c r="I42">
-        <v>0.0</v>
-      </c>
-      <c r="J42">
-        <v>0.0</v>
-      </c>
-      <c r="K42">
-        <v>28798.389466</v>
-      </c>
-      <c r="L42">
-        <v>110.864259</v>
-      </c>
-      <c r="M42">
-        <v>4370.0</v>
-      </c>
-      <c r="N42">
-        <v>1691.0</v>
-      </c>
-      <c r="O42">
-        <v>0.0</v>
-      </c>
-      <c r="P42">
-        <v>1620.0</v>
-      </c>
-      <c r="Q42">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="A43">
-        <v>7695.0</v>
-      </c>
-      <c r="B43">
-        <v>13395.0</v>
-      </c>
-      <c r="C43">
-        <v>3230.0</v>
-      </c>
-      <c r="D43">
-        <v>2850.0</v>
-      </c>
-      <c r="E43">
-        <v>8133.510534000001</v>
-      </c>
-      <c r="F43">
-        <v>0.0</v>
-      </c>
-      <c r="G43">
-        <v>0.0</v>
-      </c>
-      <c r="H43">
-        <v>0.0</v>
-      </c>
-      <c r="I43">
-        <v>0.0</v>
-      </c>
-      <c r="J43">
-        <v>0.0</v>
-      </c>
-      <c r="K43">
-        <v>27599.489466</v>
-      </c>
-      <c r="L43">
-        <v>0.0</v>
-      </c>
-      <c r="M43">
-        <v>4370.0</v>
-      </c>
-      <c r="N43">
-        <v>1691.0</v>
-      </c>
-      <c r="O43">
-        <v>0.0</v>
-      </c>
-      <c r="P43">
-        <v>1620.0</v>
-      </c>
-      <c r="Q43">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="A44">
-        <v>7695.0</v>
-      </c>
-      <c r="B44">
-        <v>13395.0</v>
-      </c>
-      <c r="C44">
-        <v>3230.0</v>
-      </c>
-      <c r="D44">
-        <v>2850.0</v>
-      </c>
-      <c r="E44">
-        <v>10106.050000000003</v>
-      </c>
-      <c r="F44">
-        <v>0.0</v>
-      </c>
-      <c r="G44">
-        <v>0.0</v>
-      </c>
-      <c r="H44">
-        <v>0.0</v>
-      </c>
-      <c r="I44">
-        <v>0.0</v>
-      </c>
-      <c r="J44">
-        <v>0.0</v>
-      </c>
-      <c r="K44">
-        <v>25523.95</v>
-      </c>
-      <c r="L44">
-        <v>0.0</v>
-      </c>
-      <c r="M44">
-        <v>4370.0</v>
-      </c>
-      <c r="N44">
-        <v>1691.0</v>
-      </c>
-      <c r="O44">
-        <v>0.0</v>
-      </c>
-      <c r="P44">
-        <v>1620.0</v>
-      </c>
-      <c r="Q44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
-      <c r="A45">
-        <v>7695.0</v>
-      </c>
-      <c r="B45">
-        <v>13395.0</v>
-      </c>
-      <c r="C45">
-        <v>3230.0</v>
-      </c>
-      <c r="D45">
-        <v>2850.0</v>
-      </c>
-      <c r="E45">
-        <v>9990.065801000004</v>
-      </c>
-      <c r="F45">
-        <v>0.0</v>
-      </c>
-      <c r="G45">
-        <v>0.0</v>
-      </c>
-      <c r="H45">
-        <v>0.0</v>
-      </c>
-      <c r="I45">
-        <v>0.0</v>
-      </c>
-      <c r="J45">
-        <v>0.0</v>
-      </c>
-      <c r="K45">
-        <v>23541.934199</v>
-      </c>
-      <c r="L45">
-        <v>0.0</v>
-      </c>
-      <c r="M45">
-        <v>4370.0</v>
-      </c>
-      <c r="N45">
-        <v>1691.0</v>
-      </c>
-      <c r="O45">
-        <v>0.0</v>
-      </c>
-      <c r="P45">
-        <v>1620.0</v>
-      </c>
-      <c r="Q45">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="A46">
-        <v>7695.0</v>
-      </c>
-      <c r="B46">
-        <v>13395.0</v>
-      </c>
-      <c r="C46">
-        <v>3230.0</v>
-      </c>
-      <c r="D46">
-        <v>2850.0</v>
-      </c>
-      <c r="E46">
-        <v>8332.389466</v>
-      </c>
-      <c r="F46">
-        <v>0.0</v>
-      </c>
-      <c r="G46">
-        <v>0.0</v>
-      </c>
-      <c r="H46">
-        <v>0.0</v>
-      </c>
-      <c r="I46">
-        <v>0.0</v>
-      </c>
-      <c r="J46">
-        <v>0.0</v>
-      </c>
-      <c r="K46">
-        <v>21681.610534</v>
-      </c>
-      <c r="L46">
-        <v>0.0</v>
-      </c>
-      <c r="M46">
-        <v>4370.0</v>
-      </c>
-      <c r="N46">
-        <v>1691.0</v>
-      </c>
-      <c r="O46">
-        <v>0.0</v>
-      </c>
-      <c r="P46">
-        <v>1620.0</v>
-      </c>
-      <c r="Q46">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="A47">
-        <v>7695.0</v>
-      </c>
-      <c r="B47">
-        <v>13395.0</v>
-      </c>
-      <c r="C47">
-        <v>3230.0</v>
-      </c>
-      <c r="D47">
-        <v>2850.0</v>
-      </c>
-      <c r="E47">
-        <v>6936.621698999996</v>
-      </c>
-      <c r="F47">
-        <v>0.0</v>
-      </c>
-      <c r="G47">
-        <v>0.0</v>
-      </c>
-      <c r="H47">
-        <v>0.0</v>
-      </c>
-      <c r="I47">
-        <v>0.0</v>
-      </c>
-      <c r="J47">
-        <v>0.0</v>
-      </c>
-      <c r="K47">
-        <v>20115.378301</v>
-      </c>
-      <c r="L47">
-        <v>0.0</v>
-      </c>
-      <c r="M47">
-        <v>4370.0</v>
-      </c>
-      <c r="N47">
-        <v>1691.0</v>
-      </c>
-      <c r="O47">
-        <v>0.0</v>
-      </c>
-      <c r="P47">
-        <v>1620.0</v>
-      </c>
-      <c r="Q47">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17">
-      <c r="A48">
-        <v>7695.0</v>
-      </c>
-      <c r="B48">
-        <v>13395.0</v>
-      </c>
-      <c r="C48">
-        <v>3230.0</v>
-      </c>
-      <c r="D48">
-        <v>2850.0</v>
-      </c>
-      <c r="E48">
-        <v>6302.257232999997</v>
-      </c>
-      <c r="F48">
-        <v>0.0</v>
-      </c>
-      <c r="G48">
-        <v>0.0</v>
-      </c>
-      <c r="H48">
-        <v>0.0</v>
-      </c>
-      <c r="I48">
-        <v>0.0</v>
-      </c>
-      <c r="J48">
-        <v>0.0</v>
-      </c>
-      <c r="K48">
-        <v>18767.742767</v>
-      </c>
-      <c r="L48">
-        <v>0.0</v>
-      </c>
-      <c r="M48">
-        <v>4370.0</v>
-      </c>
-      <c r="N48">
-        <v>1691.0</v>
-      </c>
-      <c r="O48">
-        <v>0.0</v>
-      </c>
-      <c r="P48">
-        <v>1620.0</v>
-      </c>
-      <c r="Q48">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17">
-      <c r="A49">
-        <v>7695.0</v>
-      </c>
-      <c r="B49">
-        <v>13395.0</v>
-      </c>
-      <c r="C49">
-        <v>3230.0</v>
-      </c>
-      <c r="D49">
-        <v>2850.0</v>
-      </c>
-      <c r="E49">
-        <v>3381.5980340000024</v>
-      </c>
-      <c r="F49">
-        <v>0.0</v>
-      </c>
-      <c r="G49">
-        <v>0.0</v>
-      </c>
-      <c r="H49">
-        <v>0.0</v>
-      </c>
-      <c r="I49">
-        <v>0.0</v>
-      </c>
-      <c r="J49">
-        <v>0.0</v>
-      </c>
-      <c r="K49">
-        <v>17369.401965999998</v>
-      </c>
-      <c r="L49">
-        <v>0.0</v>
-      </c>
-      <c r="M49">
-        <v>4370.0</v>
-      </c>
-      <c r="N49">
-        <v>1691.0</v>
-      </c>
-      <c r="O49">
-        <v>0.0</v>
-      </c>
-      <c r="P49">
-        <v>1620.0</v>
-      </c>
-      <c r="Q49">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Speicher eingefügt (Pumpspeicher) - funktioniert soweit. Weitere Anpassungen notwendig
</commit_message>
<xml_diff>
--- a/ErgebnisseDE.xlsx
+++ b/ErgebnisseDE.xlsx
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1122,642 +1122,6 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14">
-        <v>2167.078321000001</v>
-      </c>
-      <c r="B14">
-        <v>0.0</v>
-      </c>
-      <c r="C14">
-        <v>0.0</v>
-      </c>
-      <c r="D14">
-        <v>0.0</v>
-      </c>
-      <c r="E14">
-        <v>0.0</v>
-      </c>
-      <c r="F14">
-        <v>0.0</v>
-      </c>
-      <c r="G14">
-        <v>0.0</v>
-      </c>
-      <c r="H14">
-        <v>0.0</v>
-      </c>
-      <c r="I14">
-        <v>0.0</v>
-      </c>
-      <c r="J14">
-        <v>0.0</v>
-      </c>
-      <c r="K14">
-        <v>40451.607233</v>
-      </c>
-      <c r="L14">
-        <v>2981.314446</v>
-      </c>
-      <c r="M14">
-        <v>4370.0</v>
-      </c>
-      <c r="N14">
-        <v>1691.0</v>
-      </c>
-      <c r="O14">
-        <v>0.0</v>
-      </c>
-      <c r="P14">
-        <v>0.0</v>
-      </c>
-      <c r="Q14">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15">
-        <v>1414.5843759999989</v>
-      </c>
-      <c r="B15">
-        <v>0.0</v>
-      </c>
-      <c r="C15">
-        <v>0.0</v>
-      </c>
-      <c r="D15">
-        <v>0.0</v>
-      </c>
-      <c r="E15">
-        <v>0.0</v>
-      </c>
-      <c r="F15">
-        <v>0.0</v>
-      </c>
-      <c r="G15">
-        <v>0.0</v>
-      </c>
-      <c r="H15">
-        <v>0.0</v>
-      </c>
-      <c r="I15">
-        <v>0.0</v>
-      </c>
-      <c r="J15">
-        <v>0.0</v>
-      </c>
-      <c r="K15">
-        <v>41076.973034</v>
-      </c>
-      <c r="L15">
-        <v>2679.44259</v>
-      </c>
-      <c r="M15">
-        <v>4370.0</v>
-      </c>
-      <c r="N15">
-        <v>1691.0</v>
-      </c>
-      <c r="O15">
-        <v>0.0</v>
-      </c>
-      <c r="P15">
-        <v>0.0</v>
-      </c>
-      <c r="Q15">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16">
-        <v>1659.243171000002</v>
-      </c>
-      <c r="B16">
-        <v>0.0</v>
-      </c>
-      <c r="C16">
-        <v>0.0</v>
-      </c>
-      <c r="D16">
-        <v>0.0</v>
-      </c>
-      <c r="E16">
-        <v>0.0</v>
-      </c>
-      <c r="F16">
-        <v>0.0</v>
-      </c>
-      <c r="G16">
-        <v>0.0</v>
-      </c>
-      <c r="H16">
-        <v>0.0</v>
-      </c>
-      <c r="I16">
-        <v>0.0</v>
-      </c>
-      <c r="J16">
-        <v>0.0</v>
-      </c>
-      <c r="K16">
-        <v>41542.335534</v>
-      </c>
-      <c r="L16">
-        <v>1732.421295</v>
-      </c>
-      <c r="M16">
-        <v>4370.0</v>
-      </c>
-      <c r="N16">
-        <v>1691.0</v>
-      </c>
-      <c r="O16">
-        <v>0.0</v>
-      </c>
-      <c r="P16">
-        <v>0.0</v>
-      </c>
-      <c r="Q16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17">
-        <v>3049.680070000002</v>
-      </c>
-      <c r="B17">
-        <v>0.0</v>
-      </c>
-      <c r="C17">
-        <v>0.0</v>
-      </c>
-      <c r="D17">
-        <v>0.0</v>
-      </c>
-      <c r="E17">
-        <v>0.0</v>
-      </c>
-      <c r="F17">
-        <v>0.0</v>
-      </c>
-      <c r="G17">
-        <v>0.0</v>
-      </c>
-      <c r="H17">
-        <v>0.0</v>
-      </c>
-      <c r="I17">
-        <v>0.0</v>
-      </c>
-      <c r="J17">
-        <v>0.0</v>
-      </c>
-      <c r="K17">
-        <v>41520.926966</v>
-      </c>
-      <c r="L17">
-        <v>594.392964</v>
-      </c>
-      <c r="M17">
-        <v>4370.0</v>
-      </c>
-      <c r="N17">
-        <v>1691.0</v>
-      </c>
-      <c r="O17">
-        <v>0.0</v>
-      </c>
-      <c r="P17">
-        <v>0.0</v>
-      </c>
-      <c r="Q17">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18">
-        <v>4168.462293000004</v>
-      </c>
-      <c r="B18">
-        <v>0.0</v>
-      </c>
-      <c r="C18">
-        <v>0.0</v>
-      </c>
-      <c r="D18">
-        <v>0.0</v>
-      </c>
-      <c r="E18">
-        <v>0.0</v>
-      </c>
-      <c r="F18">
-        <v>0.0</v>
-      </c>
-      <c r="G18">
-        <v>0.0</v>
-      </c>
-      <c r="H18">
-        <v>0.0</v>
-      </c>
-      <c r="I18">
-        <v>0.0</v>
-      </c>
-      <c r="J18">
-        <v>0.0</v>
-      </c>
-      <c r="K18">
-        <v>42767.151966</v>
-      </c>
-      <c r="L18">
-        <v>29.385741</v>
-      </c>
-      <c r="M18">
-        <v>4370.0</v>
-      </c>
-      <c r="N18">
-        <v>1691.0</v>
-      </c>
-      <c r="O18">
-        <v>0.0</v>
-      </c>
-      <c r="P18">
-        <v>0.0</v>
-      </c>
-      <c r="Q18">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19">
-        <v>6695.537500000006</v>
-      </c>
-      <c r="B19">
-        <v>0.0</v>
-      </c>
-      <c r="C19">
-        <v>0.0</v>
-      </c>
-      <c r="D19">
-        <v>0.0</v>
-      </c>
-      <c r="E19">
-        <v>0.0</v>
-      </c>
-      <c r="F19">
-        <v>0.0</v>
-      </c>
-      <c r="G19">
-        <v>0.0</v>
-      </c>
-      <c r="H19">
-        <v>0.0</v>
-      </c>
-      <c r="I19">
-        <v>0.0</v>
-      </c>
-      <c r="J19">
-        <v>0.0</v>
-      </c>
-      <c r="K19">
-        <v>43436.462499999994</v>
-      </c>
-      <c r="L19">
-        <v>0.0</v>
-      </c>
-      <c r="M19">
-        <v>4370.0</v>
-      </c>
-      <c r="N19">
-        <v>1691.0</v>
-      </c>
-      <c r="O19">
-        <v>0.0</v>
-      </c>
-      <c r="P19">
-        <v>0.0</v>
-      </c>
-      <c r="Q19">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20">
-        <v>7294.946699</v>
-      </c>
-      <c r="B20">
-        <v>0.0</v>
-      </c>
-      <c r="C20">
-        <v>0.0</v>
-      </c>
-      <c r="D20">
-        <v>0.0</v>
-      </c>
-      <c r="E20">
-        <v>0.0</v>
-      </c>
-      <c r="F20">
-        <v>0.0</v>
-      </c>
-      <c r="G20">
-        <v>0.0</v>
-      </c>
-      <c r="H20">
-        <v>0.0</v>
-      </c>
-      <c r="I20">
-        <v>0.0</v>
-      </c>
-      <c r="J20">
-        <v>0.0</v>
-      </c>
-      <c r="K20">
-        <v>43415.053301</v>
-      </c>
-      <c r="L20">
-        <v>0.0</v>
-      </c>
-      <c r="M20">
-        <v>4370.0</v>
-      </c>
-      <c r="N20">
-        <v>1691.0</v>
-      </c>
-      <c r="O20">
-        <v>0.0</v>
-      </c>
-      <c r="P20">
-        <v>0.0</v>
-      </c>
-      <c r="Q20">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21">
-        <v>7090.503301000004</v>
-      </c>
-      <c r="B21">
-        <v>0.0</v>
-      </c>
-      <c r="C21">
-        <v>0.0</v>
-      </c>
-      <c r="D21">
-        <v>0.0</v>
-      </c>
-      <c r="E21">
-        <v>0.0</v>
-      </c>
-      <c r="F21">
-        <v>0.0</v>
-      </c>
-      <c r="G21">
-        <v>0.0</v>
-      </c>
-      <c r="H21">
-        <v>0.0</v>
-      </c>
-      <c r="I21">
-        <v>0.0</v>
-      </c>
-      <c r="J21">
-        <v>0.0</v>
-      </c>
-      <c r="K21">
-        <v>43063.496698999996</v>
-      </c>
-      <c r="L21">
-        <v>0.0</v>
-      </c>
-      <c r="M21">
-        <v>4370.0</v>
-      </c>
-      <c r="N21">
-        <v>1691.0</v>
-      </c>
-      <c r="O21">
-        <v>0.0</v>
-      </c>
-      <c r="P21">
-        <v>0.0</v>
-      </c>
-      <c r="Q21">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22">
-        <v>4908.165801000003</v>
-      </c>
-      <c r="B22">
-        <v>0.0</v>
-      </c>
-      <c r="C22">
-        <v>0.0</v>
-      </c>
-      <c r="D22">
-        <v>0.0</v>
-      </c>
-      <c r="E22">
-        <v>0.0</v>
-      </c>
-      <c r="F22">
-        <v>0.0</v>
-      </c>
-      <c r="G22">
-        <v>0.0</v>
-      </c>
-      <c r="H22">
-        <v>0.0</v>
-      </c>
-      <c r="I22">
-        <v>0.0</v>
-      </c>
-      <c r="J22">
-        <v>0.0</v>
-      </c>
-      <c r="K22">
-        <v>43039.834199</v>
-      </c>
-      <c r="L22">
-        <v>0.0</v>
-      </c>
-      <c r="M22">
-        <v>4370.0</v>
-      </c>
-      <c r="N22">
-        <v>1691.0</v>
-      </c>
-      <c r="O22">
-        <v>0.0</v>
-      </c>
-      <c r="P22">
-        <v>0.0</v>
-      </c>
-      <c r="Q22">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23">
-        <v>3481.684199000003</v>
-      </c>
-      <c r="B23">
-        <v>0.0</v>
-      </c>
-      <c r="C23">
-        <v>0.0</v>
-      </c>
-      <c r="D23">
-        <v>0.0</v>
-      </c>
-      <c r="E23">
-        <v>0.0</v>
-      </c>
-      <c r="F23">
-        <v>0.0</v>
-      </c>
-      <c r="G23">
-        <v>0.0</v>
-      </c>
-      <c r="H23">
-        <v>0.0</v>
-      </c>
-      <c r="I23">
-        <v>0.0</v>
-      </c>
-      <c r="J23">
-        <v>0.0</v>
-      </c>
-      <c r="K23">
-        <v>42555.315801</v>
-      </c>
-      <c r="L23">
-        <v>0.0</v>
-      </c>
-      <c r="M23">
-        <v>4370.0</v>
-      </c>
-      <c r="N23">
-        <v>1691.0</v>
-      </c>
-      <c r="O23">
-        <v>0.0</v>
-      </c>
-      <c r="P23">
-        <v>0.0</v>
-      </c>
-      <c r="Q23">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24">
-        <v>3701.8624999999956</v>
-      </c>
-      <c r="B24">
-        <v>0.0</v>
-      </c>
-      <c r="C24">
-        <v>0.0</v>
-      </c>
-      <c r="D24">
-        <v>0.0</v>
-      </c>
-      <c r="E24">
-        <v>0.0</v>
-      </c>
-      <c r="F24">
-        <v>0.0</v>
-      </c>
-      <c r="G24">
-        <v>0.0</v>
-      </c>
-      <c r="H24">
-        <v>0.0</v>
-      </c>
-      <c r="I24">
-        <v>0.0</v>
-      </c>
-      <c r="J24">
-        <v>0.0</v>
-      </c>
-      <c r="K24">
-        <v>41496.137500000004</v>
-      </c>
-      <c r="L24">
-        <v>0.0</v>
-      </c>
-      <c r="M24">
-        <v>4370.0</v>
-      </c>
-      <c r="N24">
-        <v>1691.0</v>
-      </c>
-      <c r="O24">
-        <v>0.0</v>
-      </c>
-      <c r="P24">
-        <v>0.0</v>
-      </c>
-      <c r="Q24">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25">
-        <v>1344.885534000001</v>
-      </c>
-      <c r="B25">
-        <v>0.0</v>
-      </c>
-      <c r="C25">
-        <v>0.0</v>
-      </c>
-      <c r="D25">
-        <v>0.0</v>
-      </c>
-      <c r="E25">
-        <v>0.0</v>
-      </c>
-      <c r="F25">
-        <v>0.0</v>
-      </c>
-      <c r="G25">
-        <v>0.0</v>
-      </c>
-      <c r="H25">
-        <v>0.0</v>
-      </c>
-      <c r="I25">
-        <v>0.0</v>
-      </c>
-      <c r="J25">
-        <v>0.0</v>
-      </c>
-      <c r="K25">
-        <v>41087.114466</v>
-      </c>
-      <c r="L25">
-        <v>0.0</v>
-      </c>
-      <c r="M25">
-        <v>4370.0</v>
-      </c>
-      <c r="N25">
-        <v>1691.0</v>
-      </c>
-      <c r="O25">
-        <v>0.0</v>
-      </c>
-      <c r="P25">
-        <v>0.0</v>
-      </c>
-      <c r="Q25">
-        <v>0.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>